<commit_message>
Update seed to clear PageContent
</commit_message>
<xml_diff>
--- a/public/upload/parties.xlsx
+++ b/public/upload/parties.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="29" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="14" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="184">
   <si>
     <t>ქართული ოცნება</t>
   </si>
   <si>
-    <t>ქართული ოცნება-დემოკრატიული საქართველო</t>
+    <t>ქართული ოცნება-დემოკრატიული საქართველო;საზოგადოებრივი მოძრაობა „ქართული ოცნება“</t>
   </si>
   <si>
     <t>Georgian Dream</t>
@@ -567,9 +567,6 @@
   </si>
   <si>
     <t>დემოკრატიული მოძრაობა-ერთიანი საქართველო</t>
-  </si>
-  <si>
-    <t>საზოგადოებრივი მოძრაობა „ქართული ოცნება“</t>
   </si>
 </sst>
 </file>
@@ -679,10 +676,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.2"/>
@@ -1902,12 +1899,6 @@
       <c r="K59" s="1"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C60" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D60" s="1"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
New 2016 campaign files and all related updates
</commit_message>
<xml_diff>
--- a/public/upload/parties.xlsx
+++ b/public/upload/parties.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="211">
   <si>
     <t>ქართული ოცნება</t>
   </si>
@@ -567,6 +567,87 @@
   </si>
   <si>
     <t>დემოკრატიული მოძრაობა-ერთიანი საქართველო</t>
+  </si>
+  <si>
+    <t>Democratic Movement-United Georgia</t>
+  </si>
+  <si>
+    <t>ირაკლი შიხიაშვილი დამოუკიდებელი კანდიდატი</t>
+  </si>
+  <si>
+    <t>Irakli Shikhiashvili Independent Candidate</t>
+  </si>
+  <si>
+    <t>ზვიადის გზა – უფლის სახელით</t>
+  </si>
+  <si>
+    <t>Zviadi’s Way – In the Name of the Lord</t>
+  </si>
+  <si>
+    <t>მოძრაობა-სახელმწიფო ხალხისთვის</t>
+  </si>
+  <si>
+    <t>The movement- State for People</t>
+  </si>
+  <si>
+    <t>ქალთა პარტია</t>
+  </si>
+  <si>
+    <t>Women's Party</t>
+  </si>
+  <si>
+    <t>ქართული იდეა</t>
+  </si>
+  <si>
+    <t>Georgian Idea</t>
+  </si>
+  <si>
+    <t>წარმატებული საქართველო</t>
+  </si>
+  <si>
+    <t>Successful Georgia</t>
+  </si>
+  <si>
+    <t>ჩვენი სამშობლო</t>
+  </si>
+  <si>
+    <t>Our homeland</t>
+  </si>
+  <si>
+    <t>მოქალაქეთა პოლიტიკური გაერთიანება "ახალი პოლიტიკური ცენტრი"</t>
+  </si>
+  <si>
+    <t>New Political Center</t>
+  </si>
+  <si>
+    <t>სამოქალაქო პლატფორმა – ახალი საქართველო</t>
+  </si>
+  <si>
+    <t>Civic Platform - New Georgia</t>
+  </si>
+  <si>
+    <t>სალომე ზურაბიშვილი</t>
+  </si>
+  <si>
+    <t>მოქალაქეთა პოლიტიკური გაერთიანება  „ თოფაძე -მრეწველები“</t>
+  </si>
+  <si>
+    <t>პლატფორმა ფინანსური სახელმწიფო ხალხისთვის</t>
+  </si>
+  <si>
+    <t>საარჩევნო ბლოკი   „ თოფაძე -მრეწველები, ჩვენი სამშობლო“</t>
+  </si>
+  <si>
+    <t>მამული, ენა, სარწმუნოება</t>
+  </si>
+  <si>
+    <t>ახალი პოლიტიკური მოძრაობა სახელმწიფო ხალხისთვის</t>
+  </si>
+  <si>
+    <t>პროგრესულ-დემოკრატიული მოძრაობა</t>
+  </si>
+  <si>
+    <t>საარჩევნო ბლოკი პაატა ბურჭულაძე სახელმწიფო ხალხისთვის</t>
   </si>
 </sst>
 </file>
@@ -676,10 +757,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="43.2"/>
@@ -1340,6 +1421,9 @@
       <c r="L29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>36</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>98</v>
       </c>
@@ -1533,6 +1617,9 @@
       <c r="L40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>38</v>
+      </c>
       <c r="C41" s="1" t="s">
         <v>131</v>
       </c>
@@ -1807,6 +1894,9 @@
       <c r="L54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>37</v>
+      </c>
       <c r="C55" s="1" t="s">
         <v>171</v>
       </c>
@@ -1887,10 +1977,18 @@
       <c r="L58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>34</v>
+      </c>
       <c r="C59" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="F59" s="2"/>
       <c r="G59" s="3"/>
       <c r="H59" s="1"/>
@@ -1898,6 +1996,244 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="3"/>
+    </row>
+    <row r="60" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="27.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>210</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Annual of 2016 added
</commit_message>
<xml_diff>
--- a/public/upload/parties.xlsx
+++ b/public/upload/parties.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="14" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="14"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="216">
   <si>
     <t>ქართული ოცნება</t>
   </si>
@@ -648,37 +647,36 @@
   </si>
   <si>
     <t>საარჩევნო ბლოკი პაატა ბურჭულაძე სახელმწიფო ხალხისთვის</t>
+  </si>
+  <si>
+    <t>ევროპული საქართველო</t>
+  </si>
+  <si>
+    <t>თავისუფლება ზვიად გამსახურდიას გზა</t>
+  </si>
+  <si>
+    <t>ნეიტრალური საქართველო</t>
+  </si>
+  <si>
+    <t>სრულიად საქართველოს რადიკალ-დემოკრატთა ნაციონალური პარტია</t>
+  </si>
+  <si>
+    <t>მოქალაქეთა პოლიტიკური გაერთიანება სახალხო ხელისუფლება</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -690,7 +688,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -698,87 +696,339 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:L76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="43.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.20408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.8367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="21.9336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.6224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3316326530612"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="3.140625"/>
+    <col min="2" max="2" width="41.42578125"/>
+    <col min="3" max="3" width="69.85546875"/>
+    <col min="4" max="5" width="22"/>
+    <col min="6" max="6" width="11.5703125"/>
+    <col min="7" max="7" width="10.28515625"/>
+    <col min="8" max="8" width="48.5703125"/>
+    <col min="9" max="9" width="11.28515625"/>
+    <col min="10" max="10" width="34.5703125"/>
+    <col min="11" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="n">
+    <row r="1" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -790,7 +1040,7 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2"/>
@@ -801,8 +1051,8 @@
       <c r="K1" s="1"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -825,8 +1075,8 @@
       <c r="K2" s="1"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -849,8 +1099,8 @@
       <c r="K3" s="1"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -873,8 +1123,8 @@
       <c r="K4" s="1"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -897,8 +1147,8 @@
       <c r="K5" s="1"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -921,8 +1171,8 @@
       <c r="K6" s="1"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -945,8 +1195,8 @@
       <c r="K7" s="1"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -969,8 +1219,8 @@
       <c r="K8" s="1"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>9</v>
       </c>
       <c r="B9" s="3"/>
@@ -991,8 +1241,8 @@
       <c r="K9" s="1"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1015,8 +1265,8 @@
       <c r="K10" s="1"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1039,8 +1289,8 @@
       <c r="K11" s="1"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1063,8 +1313,8 @@
       <c r="K12" s="1"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1087,8 +1337,8 @@
       <c r="K13" s="1"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1111,8 +1361,8 @@
       <c r="K14" s="1"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1135,8 +1385,8 @@
       <c r="K15" s="1"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1156,8 +1406,8 @@
       <c r="K16" s="1"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1180,8 +1430,8 @@
       <c r="K17" s="1"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1204,8 +1454,8 @@
       <c r="K18" s="1"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1228,8 +1478,8 @@
       <c r="K19" s="1"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1252,11 +1502,11 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>22</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>71</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1276,7 +1526,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>74</v>
       </c>
@@ -1294,7 +1544,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
         <v>77</v>
       </c>
@@ -1312,7 +1562,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>80</v>
       </c>
@@ -1330,7 +1580,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>83</v>
       </c>
@@ -1348,7 +1598,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>86</v>
       </c>
@@ -1366,7 +1616,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>89</v>
       </c>
@@ -1384,7 +1634,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
         <v>92</v>
       </c>
@@ -1402,7 +1652,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
         <v>95</v>
       </c>
@@ -1420,8 +1670,8 @@
       <c r="K29" s="3"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+    <row r="30" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1439,7 +1689,7 @@
       <c r="I30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
         <v>101</v>
       </c>
@@ -1457,7 +1707,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>104</v>
       </c>
@@ -1473,7 +1723,7 @@
       <c r="I32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
         <v>107</v>
       </c>
@@ -1489,7 +1739,7 @@
       <c r="I33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
         <v>110</v>
       </c>
@@ -1507,7 +1757,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
         <v>113</v>
       </c>
@@ -1525,7 +1775,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>116</v>
       </c>
@@ -1541,7 +1791,7 @@
       <c r="I36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
         <v>119</v>
       </c>
@@ -1559,7 +1809,10 @@
       <c r="K37" s="1"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>54</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>122</v>
       </c>
@@ -1577,7 +1830,7 @@
       <c r="K38" s="1"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
         <v>125</v>
       </c>
@@ -1595,8 +1848,8 @@
       <c r="K39" s="1"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+    <row r="40" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
         <v>23</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1616,8 +1869,8 @@
       <c r="K40" s="1"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+    <row r="41" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>38</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1635,8 +1888,8 @@
       <c r="I41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+    <row r="42" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
         <v>30</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1656,7 +1909,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="1" t="s">
         <v>137</v>
       </c>
@@ -1674,7 +1927,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C44" s="1" t="s">
         <v>140</v>
       </c>
@@ -1692,7 +1945,10 @@
       <c r="K44" s="1"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>55</v>
+      </c>
       <c r="B45" s="3"/>
       <c r="C45" s="1" t="s">
         <v>143</v>
@@ -1711,8 +1967,8 @@
       <c r="K45" s="1"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+    <row r="46" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
         <v>25</v>
       </c>
       <c r="B46" s="3"/>
@@ -1733,8 +1989,8 @@
       <c r="K46" s="1"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+    <row r="47" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>26</v>
       </c>
       <c r="B47" s="3"/>
@@ -1755,8 +2011,8 @@
       <c r="K47" s="1"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+    <row r="48" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>27</v>
       </c>
       <c r="B48" s="1"/>
@@ -1777,8 +2033,8 @@
       <c r="K48" s="1"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+    <row r="49" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
         <v>28</v>
       </c>
       <c r="B49" s="3"/>
@@ -1799,8 +2055,8 @@
       <c r="K49" s="1"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
+    <row r="50" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>29</v>
       </c>
       <c r="B50" s="3"/>
@@ -1821,7 +2077,7 @@
       <c r="K50" s="1"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C51" s="1" t="s">
         <v>160</v>
       </c>
@@ -1839,7 +2095,7 @@
       <c r="K51" s="1"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C52" s="1" t="s">
         <v>43</v>
       </c>
@@ -1857,7 +2113,7 @@
       <c r="K52" s="1"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C53" s="1" t="s">
         <v>165</v>
       </c>
@@ -1875,7 +2131,7 @@
       <c r="K53" s="1"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C54" s="1" t="s">
         <v>168</v>
       </c>
@@ -1893,8 +2149,8 @@
       <c r="K54" s="1"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+    <row r="55" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55">
         <v>37</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -1914,8 +2170,8 @@
       <c r="K55" s="1"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+    <row r="56" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
         <v>24</v>
       </c>
       <c r="B56" s="1"/>
@@ -1934,8 +2190,8 @@
       <c r="I56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+    <row r="57" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
         <v>31</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -1955,8 +2211,8 @@
       <c r="K57" s="1"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+    <row r="58" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
         <v>32</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -1976,8 +2232,8 @@
       <c r="K58" s="1"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
+    <row r="59" spans="1:12" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59">
         <v>34</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -1997,11 +2253,11 @@
       <c r="K59" s="1"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
+    <row r="60" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A60">
         <v>33</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" t="s">
         <v>185</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2011,11 +2267,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+    <row r="61" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A61">
         <v>35</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" t="s">
         <v>187</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -2025,11 +2281,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
+    <row r="62" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A62">
         <v>39</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" t="s">
         <v>189</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2039,11 +2295,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63">
         <v>40</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" t="s">
         <v>191</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -2053,11 +2309,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64">
         <v>41</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" t="s">
         <v>193</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2067,11 +2323,11 @@
         <v>194</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
         <v>42</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" t="s">
         <v>195</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2081,11 +2337,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
         <v>43</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" t="s">
         <v>197</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -2095,11 +2351,11 @@
         <v>198</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
         <v>44</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" t="s">
         <v>199</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2109,11 +2365,11 @@
         <v>200</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="27.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
+    <row r="68" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A68">
         <v>45</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" t="s">
         <v>201</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2123,123 +2379,162 @@
         <v>202</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69">
         <v>46</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" t="s">
         <v>203</v>
       </c>
-      <c r="D69" s="0" t="s">
+      <c r="D69" t="s">
         <v>203</v>
       </c>
-      <c r="E69" s="0" t="s">
+      <c r="E69" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70">
         <v>47</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C70" t="s">
         <v>204</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="D70" t="s">
         <v>204</v>
       </c>
-      <c r="E70" s="0" t="s">
+      <c r="E70" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71">
         <v>48</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" t="s">
         <v>205</v>
       </c>
-      <c r="D71" s="0" t="s">
+      <c r="D71" t="s">
         <v>205</v>
       </c>
-      <c r="E71" s="0" t="s">
+      <c r="E71" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72">
         <v>49</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" t="s">
         <v>206</v>
       </c>
-      <c r="D72" s="0" t="s">
+      <c r="D72" t="s">
         <v>206</v>
       </c>
-      <c r="E72" s="0" t="s">
+      <c r="E72" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73">
         <v>50</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" t="s">
         <v>207</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="D73" t="s">
         <v>207</v>
       </c>
-      <c r="E73" s="0" t="s">
+      <c r="E73" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="n">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74">
         <v>51</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="C74" t="s">
         <v>208</v>
       </c>
-      <c r="D74" s="0" t="s">
+      <c r="D74" t="s">
         <v>208</v>
       </c>
-      <c r="E74" s="0" t="s">
+      <c r="E74" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="n">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
         <v>52</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C75" t="s">
         <v>209</v>
       </c>
-      <c r="D75" s="0" t="s">
+      <c r="D75" t="s">
         <v>209</v>
       </c>
-      <c r="E75" s="0" t="s">
+      <c r="E75" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="n">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76">
         <v>53</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" t="s">
         <v>210</v>
       </c>
-      <c r="D76" s="0" t="s">
+      <c r="D76" t="s">
         <v>210</v>
       </c>
-      <c r="E76" s="0" t="s">
+      <c r="E76" t="s">
         <v>210</v>
       </c>
     </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>56</v>
+      </c>
+      <c r="C77" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>57</v>
+      </c>
+      <c r="C78" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>58</v>
+      </c>
+      <c r="C79" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>59</v>
+      </c>
+      <c r="C80" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>60</v>
+      </c>
+      <c r="C81" t="s">
+        <v>215</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>